<commit_message>
change stacked bar chart
</commit_message>
<xml_diff>
--- a/evaluation/code/BURT ICSE’22 Evaluation Survey_eleven_users.xlsx
+++ b/evaluation/code/BURT ICSE’22 Evaluation Survey_eleven_users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\burt\evaluation\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BAEB0B-0626-45BE-B1CD-09B86A252D41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B6241B-4303-4EBD-BD3C-CEE657A28B19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31519" yWindow="495" windowWidth="26438" windowHeight="14435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31922" yWindow="1267" windowWidth="24929" windowHeight="14504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet0!$A$2:$AV$14</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1379,12 +1390,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ17" sqref="AJ17"/>
+      <selection pane="bottomLeft" activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="34" max="34" width="8.796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
@@ -3287,8 +3301,9 @@
   </sheetData>
   <autoFilter ref="A2:AV14" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C1:C13 D1:D13 G1:G13 I1:I13 J1:J13 K1:K13 L1:L13 M1:M13 P1:P13 Q1:Q13 R1:R13 S1:S13 T1:T13 U1:U13 V1:V13 W1:W13 X1:X13 Y1:Y13 Z1:Z13 AA1:AA13 AB1:AB13 AC1:AC13 AD1:AD13 AE1:AE13 AF1:AF13 AG1:AG13 AH1:AH13 AI1:AI13 AJ1:AJ13 AK1:AK13 AL1:AL13 AM1:AM13 AN1:AN13 AO1:AO13 AP1:AP13 AQ1:AQ13 AR1:AR13 AS1:AS13 AT1:AT13 AU1:AU13 AV1:AV13" numberStoredAsText="1"/>
+    <ignoredError sqref="C1:C13 D1:D13 G1:G13 I1:I13 J1:J13 K1:K13 L1:L13 M1:M13 P1:P13 Q1:Q13 R1:R13 S1:S13 T1:T13 U1:U13 V1:V13 W1:W13 X1:X13 Y1:Y13 Z1:Z12 AA1:AA13 AB1:AB13 AC1:AC13 AD1:AD13 AE1:AE13 AF1:AF13 AG1:AG13 AH1:AH13 AI1:AI13 AJ1:AJ13 AK1:AK13 AL1:AL13 AM1:AM13 AN1:AN2 AO1:AO13 AP1:AP13 AQ1:AQ7 AR1 AS1:AS13 AT1:AT13 AU1:AU13 AV1:AV13 AN4:AN13 AQ10:AQ11 AQ13 AR3:AR13" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>